<commit_message>
continuação da aula 3
</commit_message>
<xml_diff>
--- a/Cia_Eletronicos.xlsx
+++ b/Cia_Eletronicos.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Dropbox\GV_2025_1S\MBA - online - Métodos e Ferramentas de Data Science\MBA online - Métodos e Ferramentas de Data Science\Aula 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabi\Documents\GitHub\mba_fgv_analytics_ia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9886FC-5C35-48DC-819F-446488D199BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEC7B8F-A5D3-4292-A7BD-1682781C09EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28035" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
     <sheet name="Perguntas" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dados!$A$1:$I$156</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1454,7 +1457,7 @@
   <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>